<commit_message>
Ajout de l'activité du jour
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_bord.xlsx
+++ b/Documentation/Journal_de_bord.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Début du projet, lire le cahier des charges du projet</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t xml:space="preserve">J'ai commencé la fonction qui me permettra d'ajouter des nouveaux articles dans la base de données </t>
+  </si>
+  <si>
+    <t>Compte rendu fait par M. Egger sur ma documentation de projet. Nous en avons discuté et j'ai commencé à améliorer les points qui sont sortis durant la disscusion</t>
+  </si>
+  <si>
+    <t>1 périodes</t>
   </si>
 </sst>
 </file>
@@ -456,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,6 +756,17 @@
         <v>1</v>
       </c>
     </row>
+    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>42796</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:C1"/>

</xml_diff>

<commit_message>
Ajout des choses dans le journal de travail
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_bord.xlsx
+++ b/Documentation/Journal_de_bord.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>Début du projet, lire le cahier des charges du projet</t>
   </si>
@@ -125,10 +125,10 @@
     <t xml:space="preserve">J'ai commencé la fonction qui me permettra d'ajouter des nouveaux articles dans la base de données </t>
   </si>
   <si>
-    <t>Compte rendu fait par M. Egger sur ma documentation de projet. Nous en avons discuté et j'ai commencé à améliorer les points qui sont sortis durant la disscusion</t>
-  </si>
-  <si>
-    <t>1 périodes</t>
+    <t>Compte rendu fait par M. Egger sur ma documentation de projet. Nous en avons discuté et j'ai commencé à améliorer les points qui sont sortis durant la disscusion. J'ai ensuite passé mon document sur un nouveau caneva qu'on nous a distribué.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai commencé à mettre des illustrations pour chaque article quand on arrive sur la page product-details.php. Ensuite j'ai commencé à faire la requête pour l'ajout des articles dans le panier. </t>
   </si>
 </sst>
 </file>
@@ -462,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,7 +756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>42796</v>
       </c>
@@ -764,7 +764,18 @@
         <v>32</v>
       </c>
       <c r="C31" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>43161</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>33</v>
+      </c>
+      <c r="C32" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rédaction du journal de travail
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_bord.xlsx
+++ b/Documentation/Journal_de_bord.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t>Début du projet, lire le cahier des charges du projet</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>Aide de M. Carrel pour une requête pour afficher l'article avec la taille qu'on a demandé de le formulaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création de la page qui permettra d'ajouter des nouveaux articles </t>
   </si>
 </sst>
 </file>
@@ -471,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,6 +816,17 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>43165</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajout de la tâche efféctuée aujourd'hui
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_bord.xlsx
+++ b/Documentation/Journal_de_bord.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
   <si>
     <t>Début du projet, lire le cahier des charges du projet</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t xml:space="preserve">Création de la page qui permettra d'ajouter des nouveaux articles </t>
+  </si>
+  <si>
+    <t>J'ai avancé la partie du code pour ajouter un article dans la base de données. Je dois encore ajouter des paramètres tels que le prix, la taille et la couleur dans la BD. Une fois que tout fonctionne je vais regarder si je peux optimiser mes requêtes.</t>
   </si>
 </sst>
 </file>
@@ -474,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,6 +831,17 @@
       </c>
       <c r="C36" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>43166</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>